<commit_message>
Fixed the goddamn bug
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t xml:space="preserve">YAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM</t>
   </si>
   <si>
     <t xml:space="preserve">IDClient</t>
@@ -161,7 +170,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -199,13 +208,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -250,6 +259,52 @@
         <v>101</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>555</v>
       </c>
     </row>
@@ -275,17 +330,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new py file and more
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -10,7 +10,6 @@
   <sheets>
     <sheet name="Employees" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Clients" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Requests" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,11 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
   <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -36,6 +38,18 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
+    <t xml:space="preserve">Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balance</t>
   </si>
   <si>
@@ -45,25 +59,13 @@
     <t xml:space="preserve">PreviousTariff</t>
   </si>
   <si>
-    <t xml:space="preserve">YAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDClient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDTariff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
+    <t xml:space="preserve">ASUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW</t>
   </si>
 </sst>
 </file>
@@ -164,13 +166,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -188,8 +190,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -211,46 +244,46 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>100</v>
@@ -264,16 +297,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>100</v>
@@ -287,16 +320,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>100</v>
@@ -306,41 +339,6 @@
       </c>
       <c r="G4" s="0" t="n">
         <v>555</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>